<commit_message>
added support for deleting people with natl
</commit_message>
<xml_diff>
--- a/js/db.xlsx
+++ b/js/db.xlsx
@@ -4105,10 +4105,10 @@
     <t>juan.vallejo.12@cnu.edu</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>8/16/2014,</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>8/16/2014,8/16/2014,8/16/2014,</t>
   </si>
   <si>
     <t>00899400</t>

</xml_diff>

<commit_message>
fixed bug that did not log event name for new participants
</commit_message>
<xml_diff>
--- a/js/db.xlsx
+++ b/js/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="1503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="1506">
   <si>
     <t>ID</t>
   </si>
@@ -4105,12 +4105,6 @@
     <t>juan.vallejo.12@cnu.edu</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Pizza My Mind (8/17/2014),Next Thursday (8/17/2014),</t>
-  </si>
-  <si>
     <t>00899400</t>
   </si>
   <si>
@@ -4523,6 +4517,21 @@
   </si>
   <si>
     <t>sanghyok.yu.14@cnu.edu</t>
+  </si>
+  <si>
+    <t>00857465</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>8/17/2014,</t>
   </si>
 </sst>
 </file>
@@ -4576,7 +4585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H434"/>
+  <dimension ref="A1:H435"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14690,21 +14699,21 @@
         <v>1362</v>
       </c>
       <c r="G389" t="s">
-        <v>1363</v>
+        <v>14</v>
       </c>
       <c r="H389" t="s">
-        <v>1364</v>
+        <v>15</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B390" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C390" t="s">
         <v>1365</v>
-      </c>
-      <c r="B390" t="s">
-        <v>1366</v>
-      </c>
-      <c r="C390" t="s">
-        <v>1367</v>
       </c>
       <c r="D390" t="s">
         <v>42</v>
@@ -14713,7 +14722,7 @@
         <v>33</v>
       </c>
       <c r="F390" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="G390" t="s">
         <v>14</v>
@@ -14724,13 +14733,13 @@
     </row>
     <row r="391">
       <c r="A391" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B391" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C391" t="s">
         <v>1369</v>
-      </c>
-      <c r="B391" t="s">
-        <v>1370</v>
-      </c>
-      <c r="C391" t="s">
-        <v>1371</v>
       </c>
       <c r="D391" t="s">
         <v>23</v>
@@ -14739,7 +14748,7 @@
         <v>12</v>
       </c>
       <c r="F391" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="G391" t="s">
         <v>14</v>
@@ -14750,10 +14759,10 @@
     </row>
     <row r="392">
       <c r="A392" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="B392" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="C392" t="s">
         <v>369</v>
@@ -14765,7 +14774,7 @@
         <v>12</v>
       </c>
       <c r="F392" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="G392" t="s">
         <v>14</v>
@@ -14776,13 +14785,13 @@
     </row>
     <row r="393">
       <c r="A393" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B393" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C393" t="s">
         <v>1376</v>
-      </c>
-      <c r="B393" t="s">
-        <v>1377</v>
-      </c>
-      <c r="C393" t="s">
-        <v>1378</v>
       </c>
       <c r="D393" t="s">
         <v>42</v>
@@ -14791,7 +14800,7 @@
         <v>12</v>
       </c>
       <c r="F393" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="G393" t="s">
         <v>14</v>
@@ -14802,10 +14811,10 @@
     </row>
     <row r="394">
       <c r="A394" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="B394" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="C394" t="s">
         <v>164</v>
@@ -14817,7 +14826,7 @@
         <v>12</v>
       </c>
       <c r="F394" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="G394" t="s">
         <v>14</v>
@@ -14828,10 +14837,10 @@
     </row>
     <row r="395">
       <c r="A395" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="B395" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="C395" t="s">
         <v>83</v>
@@ -14843,7 +14852,7 @@
         <v>12</v>
       </c>
       <c r="F395" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="G395" t="s">
         <v>14</v>
@@ -14854,7 +14863,7 @@
     </row>
     <row r="396">
       <c r="A396" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="B396" t="s">
         <v>22</v>
@@ -14869,7 +14878,7 @@
         <v>12</v>
       </c>
       <c r="F396" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="G396" t="s">
         <v>14</v>
@@ -14880,10 +14889,10 @@
     </row>
     <row r="397">
       <c r="A397" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="B397" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="C397" t="s">
         <v>883</v>
@@ -14895,7 +14904,7 @@
         <v>12</v>
       </c>
       <c r="F397" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="G397" t="s">
         <v>14</v>
@@ -14906,10 +14915,10 @@
     </row>
     <row r="398">
       <c r="A398" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="B398" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="C398" t="s">
         <v>685</v>
@@ -14921,7 +14930,7 @@
         <v>12</v>
       </c>
       <c r="F398" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="G398" t="s">
         <v>14</v>
@@ -14932,10 +14941,10 @@
     </row>
     <row r="399">
       <c r="A399" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="B399" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C399" t="s">
         <v>118</v>
@@ -14947,7 +14956,7 @@
         <v>12</v>
       </c>
       <c r="F399" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="G399" t="s">
         <v>14</v>
@@ -14958,13 +14967,13 @@
     </row>
     <row r="400">
       <c r="A400" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C400" t="s">
         <v>1396</v>
-      </c>
-      <c r="B400" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C400" t="s">
-        <v>1398</v>
       </c>
       <c r="D400" t="s">
         <v>11</v>
@@ -14973,7 +14982,7 @@
         <v>43</v>
       </c>
       <c r="F400" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="G400" t="s">
         <v>14</v>
@@ -14984,13 +14993,13 @@
     </row>
     <row r="401">
       <c r="A401" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B401" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C401" t="s">
         <v>1400</v>
-      </c>
-      <c r="B401" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C401" t="s">
-        <v>1402</v>
       </c>
       <c r="D401" t="s">
         <v>42</v>
@@ -14999,7 +15008,7 @@
         <v>12</v>
       </c>
       <c r="F401" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="G401" t="s">
         <v>14</v>
@@ -15010,10 +15019,10 @@
     </row>
     <row r="402">
       <c r="A402" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="B402" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="C402" t="s">
         <v>22</v>
@@ -15025,7 +15034,7 @@
         <v>285</v>
       </c>
       <c r="F402" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="G402" t="s">
         <v>14</v>
@@ -15036,10 +15045,10 @@
     </row>
     <row r="403">
       <c r="A403" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="B403" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="C403" t="s">
         <v>32</v>
@@ -15051,7 +15060,7 @@
         <v>12</v>
       </c>
       <c r="F403" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="G403" t="s">
         <v>14</v>
@@ -15062,10 +15071,10 @@
     </row>
     <row r="404">
       <c r="A404" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="B404" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="C404" t="s">
         <v>230</v>
@@ -15077,7 +15086,7 @@
         <v>12</v>
       </c>
       <c r="F404" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="G404" t="s">
         <v>14</v>
@@ -15088,10 +15097,10 @@
     </row>
     <row r="405">
       <c r="A405" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="B405" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="C405" t="s">
         <v>264</v>
@@ -15103,7 +15112,7 @@
         <v>12</v>
       </c>
       <c r="F405" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="G405" t="s">
         <v>14</v>
@@ -15114,13 +15123,13 @@
     </row>
     <row r="406">
       <c r="A406" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B406" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C406" t="s">
         <v>1414</v>
-      </c>
-      <c r="B406" t="s">
-        <v>1415</v>
-      </c>
-      <c r="C406" t="s">
-        <v>1416</v>
       </c>
       <c r="D406" t="s">
         <v>42</v>
@@ -15129,7 +15138,7 @@
         <v>12</v>
       </c>
       <c r="F406" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="G406" t="s">
         <v>14</v>
@@ -15140,10 +15149,10 @@
     </row>
     <row r="407">
       <c r="A407" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="B407" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="C407" t="s">
         <v>32</v>
@@ -15155,7 +15164,7 @@
         <v>285</v>
       </c>
       <c r="F407" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="G407" t="s">
         <v>14</v>
@@ -15166,13 +15175,13 @@
     </row>
     <row r="408">
       <c r="A408" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="B408" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="C408" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="D408" t="s">
         <v>42</v>
@@ -15181,7 +15190,7 @@
         <v>12</v>
       </c>
       <c r="F408" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="G408" t="s">
         <v>14</v>
@@ -15192,10 +15201,10 @@
     </row>
     <row r="409">
       <c r="A409" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="B409" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="C409" t="s">
         <v>827</v>
@@ -15207,7 +15216,7 @@
         <v>12</v>
       </c>
       <c r="F409" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="G409" t="s">
         <v>14</v>
@@ -15218,10 +15227,10 @@
     </row>
     <row r="410">
       <c r="A410" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="B410" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="C410" t="s">
         <v>1295</v>
@@ -15233,7 +15242,7 @@
         <v>12</v>
       </c>
       <c r="F410" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="G410" t="s">
         <v>14</v>
@@ -15244,10 +15253,10 @@
     </row>
     <row r="411">
       <c r="A411" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="B411" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="C411" t="s">
         <v>222</v>
@@ -15259,7 +15268,7 @@
         <v>28</v>
       </c>
       <c r="F411" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="G411" t="s">
         <v>14</v>
@@ -15270,10 +15279,10 @@
     </row>
     <row r="412">
       <c r="A412" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="B412" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="C412" t="s">
         <v>134</v>
@@ -15285,7 +15294,7 @@
         <v>12</v>
       </c>
       <c r="F412" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="G412" t="s">
         <v>14</v>
@@ -15296,10 +15305,10 @@
     </row>
     <row r="413">
       <c r="A413" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="B413" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="C413" t="s">
         <v>32</v>
@@ -15311,7 +15320,7 @@
         <v>28</v>
       </c>
       <c r="F413" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="G413" t="s">
         <v>14</v>
@@ -15322,10 +15331,10 @@
     </row>
     <row r="414">
       <c r="A414" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B414" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="C414" t="s">
         <v>168</v>
@@ -15337,7 +15346,7 @@
         <v>12</v>
       </c>
       <c r="F414" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="G414" t="s">
         <v>14</v>
@@ -15348,10 +15357,10 @@
     </row>
     <row r="415">
       <c r="A415" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="B415" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="C415" t="s">
         <v>226</v>
@@ -15363,7 +15372,7 @@
         <v>12</v>
       </c>
       <c r="F415" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="G415" t="s">
         <v>14</v>
@@ -15374,10 +15383,10 @@
     </row>
     <row r="416">
       <c r="A416" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="B416" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="C416" t="s">
         <v>845</v>
@@ -15389,7 +15398,7 @@
         <v>12</v>
       </c>
       <c r="F416" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="G416" t="s">
         <v>14</v>
@@ -15400,10 +15409,10 @@
     </row>
     <row r="417">
       <c r="A417" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="B417" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="C417" t="s">
         <v>134</v>
@@ -15415,7 +15424,7 @@
         <v>24</v>
       </c>
       <c r="F417" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="G417" t="s">
         <v>14</v>
@@ -15426,10 +15435,10 @@
     </row>
     <row r="418">
       <c r="A418" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="B418" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="C418" t="s">
         <v>134</v>
@@ -15441,7 +15450,7 @@
         <v>33</v>
       </c>
       <c r="F418" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="G418" t="s">
         <v>14</v>
@@ -15452,7 +15461,7 @@
     </row>
     <row r="419">
       <c r="A419" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="B419" t="s">
         <v>299</v>
@@ -15467,7 +15476,7 @@
         <v>28</v>
       </c>
       <c r="F419" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="G419" t="s">
         <v>14</v>
@@ -15478,10 +15487,10 @@
     </row>
     <row r="420">
       <c r="A420" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B420" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C420" t="s">
         <v>10</v>
@@ -15493,7 +15502,7 @@
         <v>33</v>
       </c>
       <c r="F420" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="G420" t="s">
         <v>14</v>
@@ -15504,10 +15513,10 @@
     </row>
     <row r="421">
       <c r="A421" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="B421" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="C421" t="s">
         <v>195</v>
@@ -15519,7 +15528,7 @@
         <v>12</v>
       </c>
       <c r="F421" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="G421" t="s">
         <v>14</v>
@@ -15530,13 +15539,13 @@
     </row>
     <row r="422">
       <c r="A422" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="B422" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="C422" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="D422" t="s">
         <v>11</v>
@@ -15545,7 +15554,7 @@
         <v>43</v>
       </c>
       <c r="F422" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="G422" t="s">
         <v>14</v>
@@ -15556,10 +15565,10 @@
     </row>
     <row r="423">
       <c r="A423" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="B423" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="C423" t="s">
         <v>32</v>
@@ -15571,7 +15580,7 @@
         <v>43</v>
       </c>
       <c r="F423" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="G423" t="s">
         <v>14</v>
@@ -15582,10 +15591,10 @@
     </row>
     <row r="424">
       <c r="A424" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="B424" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="C424" t="s">
         <v>279</v>
@@ -15597,7 +15606,7 @@
         <v>43</v>
       </c>
       <c r="F424" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="G424" t="s">
         <v>14</v>
@@ -15608,10 +15617,10 @@
     </row>
     <row r="425">
       <c r="A425" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="B425" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="C425" t="s">
         <v>260</v>
@@ -15623,7 +15632,7 @@
         <v>12</v>
       </c>
       <c r="F425" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="G425" t="s">
         <v>14</v>
@@ -15634,10 +15643,10 @@
     </row>
     <row r="426">
       <c r="A426" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="B426" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="C426" t="s">
         <v>226</v>
@@ -15649,7 +15658,7 @@
         <v>33</v>
       </c>
       <c r="F426" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="G426" t="s">
         <v>14</v>
@@ -15660,10 +15669,10 @@
     </row>
     <row r="427">
       <c r="A427" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="B427" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="C427" t="s">
         <v>883</v>
@@ -15675,7 +15684,7 @@
         <v>33</v>
       </c>
       <c r="F427" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G427" t="s">
         <v>14</v>
@@ -15686,10 +15695,10 @@
     </row>
     <row r="428">
       <c r="A428" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B428" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="C428" t="s">
         <v>41</v>
@@ -15701,7 +15710,7 @@
         <v>12</v>
       </c>
       <c r="F428" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="G428" t="s">
         <v>14</v>
@@ -15712,13 +15721,13 @@
     </row>
     <row r="429">
       <c r="A429" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B429" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C429" t="s">
         <v>1481</v>
-      </c>
-      <c r="B429" t="s">
-        <v>1482</v>
-      </c>
-      <c r="C429" t="s">
-        <v>1483</v>
       </c>
       <c r="D429" t="s">
         <v>42</v>
@@ -15727,7 +15736,7 @@
         <v>33</v>
       </c>
       <c r="F429" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="G429" t="s">
         <v>14</v>
@@ -15738,13 +15747,13 @@
     </row>
     <row r="430">
       <c r="A430" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B430" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C430" t="s">
         <v>1485</v>
-      </c>
-      <c r="B430" t="s">
-        <v>1486</v>
-      </c>
-      <c r="C430" t="s">
-        <v>1487</v>
       </c>
       <c r="D430" t="s">
         <v>42</v>
@@ -15753,7 +15762,7 @@
         <v>12</v>
       </c>
       <c r="F430" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="G430" t="s">
         <v>14</v>
@@ -15764,10 +15773,10 @@
     </row>
     <row r="431">
       <c r="A431" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="B431" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="C431" t="s">
         <v>1295</v>
@@ -15779,7 +15788,7 @@
         <v>33</v>
       </c>
       <c r="F431" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="G431" t="s">
         <v>14</v>
@@ -15790,13 +15799,13 @@
     </row>
     <row r="432">
       <c r="A432" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C432" t="s">
         <v>1492</v>
-      </c>
-      <c r="B432" t="s">
-        <v>1493</v>
-      </c>
-      <c r="C432" t="s">
-        <v>1494</v>
       </c>
       <c r="D432" t="s">
         <v>19</v>
@@ -15805,7 +15814,7 @@
         <v>33</v>
       </c>
       <c r="F432" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="G432" t="s">
         <v>14</v>
@@ -15816,10 +15825,10 @@
     </row>
     <row r="433">
       <c r="A433" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="B433" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="C433" t="s">
         <v>122</v>
@@ -15831,7 +15840,7 @@
         <v>12</v>
       </c>
       <c r="F433" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="G433" t="s">
         <v>14</v>
@@ -15842,13 +15851,13 @@
     </row>
     <row r="434">
       <c r="A434" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B434" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C434" t="s">
         <v>1499</v>
-      </c>
-      <c r="B434" t="s">
-        <v>1500</v>
-      </c>
-      <c r="C434" t="s">
-        <v>1501</v>
       </c>
       <c r="D434" t="s">
         <v>11</v>
@@ -15857,13 +15866,39 @@
         <v>12</v>
       </c>
       <c r="F434" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G434" t="s">
+        <v>14</v>
+      </c>
+      <c r="H434" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B435" t="s">
         <v>1502</v>
       </c>
-      <c r="G434" t="s">
-        <v>14</v>
-      </c>
-      <c r="H434" t="s">
-        <v>15</v>
+      <c r="C435" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D435" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E435" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F435" t="s">
+        <v>1503</v>
+      </c>
+      <c r="G435" t="s">
+        <v>1504</v>
+      </c>
+      <c r="H435" t="s">
+        <v>1505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating scanner.js and database file
</commit_message>
<xml_diff>
--- a/js/db.xlsx
+++ b/js/db.xlsx
@@ -4901,11 +4901,11 @@
     <xf numFmtId="0" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -6157,14 +6157,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G472"/>
+  <dimension ref="A1:G462"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.0547" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.375" style="1" customWidth="1"/>
@@ -16798,96 +16798,6 @@
       <c r="G462" t="s" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="463" ht="18" customHeight="1">
-      <c r="A463" s="9"/>
-      <c r="B463" s="9"/>
-      <c r="C463" s="9"/>
-      <c r="D463" s="9"/>
-      <c r="E463" s="9"/>
-      <c r="F463" s="9"/>
-      <c r="G463" s="9"/>
-    </row>
-    <row r="464" ht="18" customHeight="1">
-      <c r="A464" s="9"/>
-      <c r="B464" s="9"/>
-      <c r="C464" s="9"/>
-      <c r="D464" s="9"/>
-      <c r="E464" s="9"/>
-      <c r="F464" s="9"/>
-      <c r="G464" s="9"/>
-    </row>
-    <row r="465" ht="18" customHeight="1">
-      <c r="A465" s="9"/>
-      <c r="B465" s="9"/>
-      <c r="C465" s="9"/>
-      <c r="D465" s="9"/>
-      <c r="E465" s="9"/>
-      <c r="F465" s="9"/>
-      <c r="G465" s="9"/>
-    </row>
-    <row r="466" ht="18" customHeight="1">
-      <c r="A466" s="9"/>
-      <c r="B466" s="9"/>
-      <c r="C466" s="9"/>
-      <c r="D466" s="9"/>
-      <c r="E466" s="9"/>
-      <c r="F466" s="9"/>
-      <c r="G466" s="9"/>
-    </row>
-    <row r="467" ht="18" customHeight="1">
-      <c r="A467" s="9"/>
-      <c r="B467" s="9"/>
-      <c r="C467" s="9"/>
-      <c r="D467" s="9"/>
-      <c r="E467" s="9"/>
-      <c r="F467" s="9"/>
-      <c r="G467" s="9"/>
-    </row>
-    <row r="468" ht="18" customHeight="1">
-      <c r="A468" s="9"/>
-      <c r="B468" s="9"/>
-      <c r="C468" s="9"/>
-      <c r="D468" s="9"/>
-      <c r="E468" s="9"/>
-      <c r="F468" s="9"/>
-      <c r="G468" s="9"/>
-    </row>
-    <row r="469" ht="18" customHeight="1">
-      <c r="A469" s="9"/>
-      <c r="B469" s="9"/>
-      <c r="C469" s="9"/>
-      <c r="D469" s="9"/>
-      <c r="E469" s="9"/>
-      <c r="F469" s="9"/>
-      <c r="G469" s="9"/>
-    </row>
-    <row r="470" ht="18" customHeight="1">
-      <c r="A470" s="9"/>
-      <c r="B470" s="9"/>
-      <c r="C470" s="9"/>
-      <c r="D470" s="9"/>
-      <c r="E470" s="9"/>
-      <c r="F470" s="9"/>
-      <c r="G470" s="9"/>
-    </row>
-    <row r="471" ht="18" customHeight="1">
-      <c r="A471" s="9"/>
-      <c r="B471" s="9"/>
-      <c r="C471" s="9"/>
-      <c r="D471" s="9"/>
-      <c r="E471" s="9"/>
-      <c r="F471" s="9"/>
-      <c r="G471" s="9"/>
-    </row>
-    <row r="472" ht="18" customHeight="1">
-      <c r="A472" s="9"/>
-      <c r="B472" s="9"/>
-      <c r="C472" s="9"/>
-      <c r="D472" s="9"/>
-      <c r="E472" s="9"/>
-      <c r="F472" s="9"/>
-      <c r="G472" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16906,83 +16816,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="10" customWidth="1"/>
-    <col min="6" max="256" width="6.625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="6.625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="9" customWidth="1"/>
+    <col min="6" max="256" width="6.625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" ht="15.55" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" ht="15.55" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" ht="15.55" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="15.55" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="15.55" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="15.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="15.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="15.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="15.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17010,74 +16920,74 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" ht="15.55" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" ht="15.55" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" ht="15.55" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="15.55" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="15.55" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="15.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="15.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="15.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="15.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>